<commit_message>
Fixed clients class, so it works with % instead of decimals.
</commit_message>
<xml_diff>
--- a/clients.xlsx
+++ b/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Everyday_Snacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26D3E79-85B5-4C4A-B47D-EEE259FD0B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A7DE4D-DA8F-480C-B399-BE86104575FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>MNO Vending</t>
+  </si>
+  <si>
+    <t>5%</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>3%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>7%</t>
   </si>
 </sst>
 </file>
@@ -92,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -376,7 +397,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,14 +431,14 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.02</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -427,14 +448,14 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.02</v>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -444,14 +465,14 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.03</v>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -461,14 +482,14 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.05</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -478,14 +499,14 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E6" s="1">
-        <v>7.0000000000000007E-2</v>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>